<commit_message>
worked on efficacy and effiency comparison graphs
</commit_message>
<xml_diff>
--- a/experimental_data.xlsx
+++ b/experimental_data.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Experimental Results" sheetId="1" r:id="rId1"/>
+    <sheet name="Efficacy" sheetId="3" r:id="rId2"/>
+    <sheet name="Efficacy Ratios" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="18">
   <si>
     <t>Test</t>
   </si>
@@ -75,6 +77,9 @@
   </si>
   <si>
     <t>Avg</t>
+  </si>
+  <si>
+    <t>Ratios</t>
   </si>
 </sst>
 </file>
@@ -257,6 +262,2357 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Average</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Route Length Results Over Multiple Problem Instances of Different Sizes</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Experimental Results'!$N$30:$O$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nearest Neighbour Basic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Experimental Results'!$M$32:$M$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>493</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1060</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2103</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3795</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5915</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Experimental Results'!$O$32:$O$40</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>8980.9182793291875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>825.24232272774384</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54669.0264149633</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3241.4668367219497</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43646.373961317106</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>296543.88905721199</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90517.890018195598</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="#,##0.00">
+                  <c:v>35362.50655728639</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0.00">
+                  <c:v>707498.63075170584</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-9146-4D7A-9524-739D5CCE12FC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Experimental Results'!$P$30:$Q$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nearest Neighbour Enhanced</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Experimental Results'!$M$32:$M$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>493</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1060</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2103</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3795</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5915</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Experimental Results'!$Q$32:$Q$40</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>8883.0950262112092</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>759.49701284547768</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50251.965517615645</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2920.3262210856929</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41982.406971895092</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>281530.52104881068</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>87664.56789116397</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="#,##0.00">
+                  <c:v>34226.093401388047</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0.00">
+                  <c:v>672798.02977894177</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-9146-4D7A-9524-739D5CCE12FC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="551402712"/>
+        <c:axId val="551403040"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="551402712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> of Cities, n</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="551403040"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="551403040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Route Length / units</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="6.2743854710922892E-2"/>
+              <c:y val="0.37432764218582404"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="551402712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="0"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Comparing the Algorithm's Average Route Length Results Over Problem Instances of Different Sizes</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Experimental Results'!$N$43:$O$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nearest Neighbour Basic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Experimental Results'!$M$45:$M$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>493</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1060</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2103</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3795</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5915</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Experimental Results'!$O$45:$O$53</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-5791-46FC-80E1-DF2780C7330B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Experimental Results'!$P$43:$Q$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nearest Neighbour Enhanced</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Experimental Results'!$Q$45:$Q$53</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.98910765580139703</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.92033211570517548</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91920359320431078</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90092737892668928</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96187616889098848</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.94937218886508634</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.96847781000575617</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.96786389691982433</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.95095311925071113</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-5791-46FC-80E1-DF2780C7330B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="362678392"/>
+        <c:axId val="362678720"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="362678392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:rPr>
+                  <a:t>Number of Cities, n</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="362678720"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="362678720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" rtl="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:rPr>
+                  <a:t>Route Length / units</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="362678392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="129" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="129" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9310872" cy="6084186"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9310872" cy="6084186"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -522,10 +2878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W42"/>
+  <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="P47" sqref="P47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2628,9 +4984,234 @@
         <f>AVERAGE(E32:E41)</f>
         <v>672798.02977894177</v>
       </c>
+      <c r="N42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N43" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O43" s="3"/>
+      <c r="P43" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q43" s="2"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M44" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="N44" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="O44" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="P44" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q44" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M45" s="14">
+        <v>52</v>
+      </c>
+      <c r="N45" s="18">
+        <f>N32/N32</f>
+        <v>1</v>
+      </c>
+      <c r="O45" s="18">
+        <f>O32/O32</f>
+        <v>1</v>
+      </c>
+      <c r="P45" s="18">
+        <f>P32/N32</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="Q45" s="15">
+        <f>Q32/O32</f>
+        <v>0.98910765580139703</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M46" s="8">
+        <v>101</v>
+      </c>
+      <c r="N46" s="18">
+        <f t="shared" ref="N46:N53" si="0">N33/N33</f>
+        <v>1</v>
+      </c>
+      <c r="O46" s="18">
+        <f t="shared" ref="O46:O53" si="1">O33/O33</f>
+        <v>1</v>
+      </c>
+      <c r="P46" s="18">
+        <f t="shared" ref="P46:P53" si="2">P33/N33</f>
+        <v>2.5</v>
+      </c>
+      <c r="Q46" s="15">
+        <f t="shared" ref="Q46:Q53" si="3">Q33/O33</f>
+        <v>0.92033211570517548</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M47" s="8">
+        <v>159</v>
+      </c>
+      <c r="N47" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O47" s="18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P47" s="18">
+        <f t="shared" si="2"/>
+        <v>3.4999999999999996</v>
+      </c>
+      <c r="Q47" s="15">
+        <f t="shared" si="3"/>
+        <v>0.91920359320431078</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M48" s="8">
+        <v>262</v>
+      </c>
+      <c r="N48" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O48" s="18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P48" s="18">
+        <f t="shared" si="2"/>
+        <v>3.4310344827586206</v>
+      </c>
+      <c r="Q48" s="15">
+        <f t="shared" si="3"/>
+        <v>0.90092737892668928</v>
+      </c>
+    </row>
+    <row r="49" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="M49" s="8">
+        <v>493</v>
+      </c>
+      <c r="N49" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O49" s="18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P49" s="18">
+        <f t="shared" si="2"/>
+        <v>25.510204081632651</v>
+      </c>
+      <c r="Q49" s="15">
+        <f t="shared" si="3"/>
+        <v>0.96187616889098848</v>
+      </c>
+    </row>
+    <row r="50" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="M50" s="8">
+        <v>1060</v>
+      </c>
+      <c r="N50" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O50" s="18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P50" s="18">
+        <f t="shared" si="2"/>
+        <v>82.887218045112789</v>
+      </c>
+      <c r="Q50" s="15">
+        <f t="shared" si="3"/>
+        <v>0.94937218886508634</v>
+      </c>
+    </row>
+    <row r="51" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="M51" s="8">
+        <v>2103</v>
+      </c>
+      <c r="N51" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O51" s="18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P51" s="18">
+        <f t="shared" si="2"/>
+        <v>183.55429864253392</v>
+      </c>
+      <c r="Q51" s="15">
+        <f t="shared" si="3"/>
+        <v>0.96847781000575617</v>
+      </c>
+    </row>
+    <row r="52" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="M52" s="8">
+        <v>3795</v>
+      </c>
+      <c r="N52" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O52" s="18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P52" s="18">
+        <f t="shared" si="2"/>
+        <v>335.14952589350838</v>
+      </c>
+      <c r="Q52" s="15">
+        <f t="shared" si="3"/>
+        <v>0.96786389691982433</v>
+      </c>
+    </row>
+    <row r="53" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="M53" s="8">
+        <v>5915</v>
+      </c>
+      <c r="N53" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O53" s="18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P53" s="18">
+        <f t="shared" si="2"/>
+        <v>534.37425683709876</v>
+      </c>
+      <c r="Q53" s="15">
+        <f t="shared" si="3"/>
+        <v>0.95095311925071113</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="33">
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="P43:Q43"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="B16:C16"/>

</xml_diff>

<commit_message>
more graphs (also, excel? go die.)
</commit_message>
<xml_diff>
--- a/experimental_data.xlsx
+++ b/experimental_data.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="Experimental Results" sheetId="1" r:id="rId1"/>
     <sheet name="Efficacy" sheetId="3" r:id="rId2"/>
     <sheet name="Efficacy Ratios" sheetId="4" r:id="rId3"/>
+    <sheet name="Efficiency" sheetId="5" r:id="rId4"/>
+    <sheet name="Efficiency Ratios" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -908,19 +910,17 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
+                  <a:srgbClr val="595959"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:effectLst/>
               </a:rPr>
-              <a:t>Comparing the Algorithm's Average Route Length Results Over Problem Instances of Different Sizes</a:t>
+              <a:t>Average Route Length Results as a Ratio</a:t>
             </a:r>
+            <a:endParaRPr lang="en-GB" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1263,6 +1263,8 @@
         <c:axId val="362678720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1.05"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1453,6 +1455,1178 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Average Run Time of Algorithm Over Multiple Problem Instances of Different Sizes</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Experimental Results'!$N$30:$O$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nearest Neighbour Basic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Experimental Results'!$M$32:$M$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>493</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1060</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2103</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3795</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5915</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Experimental Results'!$N$32:$N$40</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>137.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>336.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-DFB6-40FA-A331-1C442973F08F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Experimental Results'!$P$30:$Q$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nearest Neighbour Enhanced</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Experimental Results'!$M$32:$M$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>493</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1060</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2103</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3795</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5915</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Experimental Results'!$P$32:$P$40</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1102.4000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8113.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45949</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>179763.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-DFB6-40FA-A331-1C442973F08F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="233756432"/>
+        <c:axId val="559601120"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="233756432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of Cities, n</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="559601120"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="559601120"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Run</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Time / ms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="233756432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Experimental Results'!$N$43:$O$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nearest Neighbour Basic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Experimental Results'!$M$45:$M$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>493</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1060</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2103</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3795</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5915</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Experimental Results'!$N$45:$N$53</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-DA9D-4A5A-84A6-B1BEC075C3EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Experimental Results'!$P$43:$Q$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nearest Neighbour Enhanced</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Experimental Results'!$M$45:$M$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>493</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1060</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2103</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3795</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5915</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Experimental Results'!$P$45:$P$53</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.6666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4310344827586206</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.510204081632651</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>82.887218045112789</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>183.55429864253392</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>335.14952589350838</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>534.37425683709876</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-DA9D-4A5A-84A6-B1BEC075C3EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="552217048"/>
+        <c:axId val="552218688"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="552217048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="552218688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="552218688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="552217048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1533,6 +2707,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2037,6 +3291,1012 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2554,7 +4814,29 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="129" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="129" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="129" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="129" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2589,6 +4871,60 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9310872" cy="6084186"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9310872" cy="6084186"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -2880,8 +5216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="P47" sqref="P47"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2891,8 +5227,7 @@
     <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -5040,6 +7375,33 @@
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>52</v>
+      </c>
+      <c r="B46">
+        <v>101</v>
+      </c>
+      <c r="C46">
+        <v>159</v>
+      </c>
+      <c r="D46">
+        <v>262</v>
+      </c>
+      <c r="E46">
+        <v>493</v>
+      </c>
+      <c r="F46" s="8">
+        <v>1060</v>
+      </c>
+      <c r="G46" s="8">
+        <v>2103</v>
+      </c>
+      <c r="H46" s="8">
+        <v>3795</v>
+      </c>
+      <c r="I46" s="8">
+        <v>5915</v>
+      </c>
       <c r="M46" s="8">
         <v>101</v>
       </c>
@@ -5061,6 +7423,33 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>0.6</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>1.6</v>
+      </c>
+      <c r="D47">
+        <v>5.8</v>
+      </c>
+      <c r="E47">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F47">
+        <v>13.3</v>
+      </c>
+      <c r="G47">
+        <v>44.2</v>
+      </c>
+      <c r="H47">
+        <v>137.1</v>
+      </c>
+      <c r="I47">
+        <v>336.4</v>
+      </c>
       <c r="M47" s="8">
         <v>159</v>
       </c>

</xml_diff>